<commit_message>
Update NSLS Certificate Signing Request Form.xlsx
</commit_message>
<xml_diff>
--- a/Forms/NSLS Certificate Signing Request Form.xlsx
+++ b/Forms/NSLS Certificate Signing Request Form.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://novascotia.sharepoint.com/sites/DigitalPlatforms215/Shared Documents/Identity/Operations/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Digital Platform Services\Digital Identity\NS Login System\Documentation\MyNSID-Continuous-Improvement\GitHub\Nova-Scotia-Login-Service\Nova-Scotia-Login-Service\Forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="260" documentId="8_{64088184-79BD-441D-8D98-249DE76CC67A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{08891841-401F-4484-A037-35B6D9205AD1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D29F2AC-B1BD-4E5E-BCC3-52CA92578107}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="-120" windowWidth="27960" windowHeight="18240" xr2:uid="{DA2C516E-38FA-41D5-A805-320A7FF1D643}"/>
+    <workbookView xWindow="6525" yWindow="765" windowWidth="15270" windowHeight="14145" xr2:uid="{DA2C516E-38FA-41D5-A805-320A7FF1D643}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Application Information</t>
   </si>
@@ -48,9 +48,6 @@
     <t xml:space="preserve">Environment [-select one-]  </t>
   </si>
   <si>
-    <t>Business Contact (Internal)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Name  </t>
   </si>
   <si>
@@ -61,9 +58,6 @@
   </si>
   <si>
     <t xml:space="preserve">Phone  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dept. / Agency / Vendor Name  </t>
   </si>
   <si>
     <t>Production</t>
@@ -97,6 +91,18 @@
   <si>
     <t xml:space="preserve">
 NSLS Certificate Signing Request Form</t>
+  </si>
+  <si>
+    <t>Business Sponsor (GNS/NSHA)</t>
+  </si>
+  <si>
+    <t>Department  / Agency</t>
+  </si>
+  <si>
+    <t>Business Contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Department / Agency /Vendor Name  </t>
   </si>
 </sst>
 </file>
@@ -786,22 +792,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E605552-92D0-4CA8-9EB4-94C5770B000C}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="40" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.85546875" style="1" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B1" s="22"/>
       <c r="F1" s="16"/>
@@ -833,61 +839,91 @@
     <row r="6" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="9" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="17"/>
+    </row>
+    <row r="9" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="17"/>
+    </row>
+    <row r="10" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="17"/>
+    </row>
+    <row r="13" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="17"/>
+    </row>
+    <row r="14" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="17"/>
-    </row>
-    <row r="9" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="9" t="s">
+    </row>
+    <row r="15" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="18"/>
+    </row>
+    <row r="17" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="18"/>
-    </row>
-    <row r="12" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="8"/>
-    </row>
-    <row r="13" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="7"/>
-    </row>
-    <row r="14" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="20"/>
+      <c r="B17" s="8"/>
+    </row>
+    <row r="18" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="7"/>
+    </row>
+    <row r="19" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A20:B20"/>
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -923,12 +959,12 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -943,6 +979,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C3DA4F9BC48E6749B7F6096675E736D4" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0dd3fa7870eaff2fa578fd9b3523f5d9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d4b32c5d-14cc-49d4-8e33-89dfffb4ed54" xmlns:ns3="cf40fa3a-ca34-444b-baec-089d050d3c0a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8963a769a5b2d572f5b9b7e76b18efa4" ns2:_="" ns3:_="">
     <xsd:import namespace="d4b32c5d-14cc-49d4-8e33-89dfffb4ed54"/>
@@ -1153,15 +1198,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4343B8F1-1454-4983-A8D9-69E52EB922A3}">
   <ds:schemaRefs>
@@ -1180,6 +1216,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16145780-3408-4614-9F7D-E9BC72CB2CD0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE2FA794-B4E7-464D-96E2-97F3C6D8DE95}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1196,12 +1240,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16145780-3408-4614-9F7D-E9BC72CB2CD0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Remove expired IdP metadata XML
</commit_message>
<xml_diff>
--- a/Forms/NSLS Certificate Signing Request Form.xlsx
+++ b/Forms/NSLS Certificate Signing Request Form.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Digital Platform Services\Digital Identity\NS Login System\Documentation\MyNSID-Continuous-Improvement\GitHub\Nova-Scotia-Login-Service\Nova-Scotia-Login-Service\Forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Digital Platform Services\Digital Identity\MyNSID\Documentation\MyNSID-Continuous-Improvement\GitHub\Nova-Scotia-Login-Service\Nova-Scotia-Login-System\Forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5AADF7-3526-4F2E-85E6-C5F0E8227D01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8098AB2-EE27-48DB-BC4A-9EDFBB54B9DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="2355" windowWidth="14520" windowHeight="12945" xr2:uid="{DA2C516E-38FA-41D5-A805-320A7FF1D643}"/>
+    <workbookView xWindow="960" yWindow="-120" windowWidth="27960" windowHeight="18240" xr2:uid="{DA2C516E-38FA-41D5-A805-320A7FF1D643}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Application Information</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t xml:space="preserve">Support Group/Vendor Name  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Classification (A, B, C..) </t>
   </si>
 </sst>
 </file>
@@ -783,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E605552-92D0-4CA8-9EB4-94C5770B000C}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -817,98 +820,104 @@
     </row>
     <row r="4" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6"/>
-    </row>
-    <row r="5" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="16"/>
-    </row>
-    <row r="8" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="B8" s="16"/>
+    </row>
+    <row r="9" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="16"/>
-    </row>
-    <row r="12" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="B12" s="16"/>
+    </row>
+    <row r="13" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="4"/>
-    </row>
-    <row r="13" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="16"/>
-    </row>
-    <row r="16" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="8"/>
+      <c r="B16" s="16"/>
     </row>
     <row r="17" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="8"/>
+    </row>
+    <row r="18" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="7"/>
-    </row>
-    <row r="18" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
+      <c r="B18" s="7"/>
+    </row>
+    <row r="19" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:2" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B19" s="18"/>
+      <c r="B20" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -921,7 +930,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B4</xm:sqref>
+          <xm:sqref>B5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1167,18 +1176,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1201,6 +1210,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16145780-3408-4614-9F7D-E9BC72CB2CD0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4343B8F1-1454-4983-A8D9-69E52EB922A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="d4b32c5d-14cc-49d4-8e33-89dfffb4ed54"/>
@@ -1215,12 +1232,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16145780-3408-4614-9F7D-E9BC72CB2CD0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>